<commit_message>
Standalone application updated without warning messages
</commit_message>
<xml_diff>
--- a/PVBatterySystem/for_redistribution_files_only/economicanalysis.xlsx
+++ b/PVBatterySystem/for_redistribution_files_only/economicanalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\NREL\PVTesBattery\PVBatterySystem\for_redistribution_files_only\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4916676A-4CE5-4FC2-A752-FE15C0D247EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C0C8F3-66E3-461E-974E-D142CF5ADEE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="17280" windowHeight="9030" firstSheet="4" activeTab="7" xr2:uid="{A1D91E46-10FA-4AC4-B06A-F6A502160249}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="17280" windowHeight="9030" firstSheet="4" activeTab="7" xr2:uid="{A1D91E46-10FA-4AC4-B06A-F6A502160249}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOE System" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated standalone app accounting for warning message change
</commit_message>
<xml_diff>
--- a/PVBatterySystem/for_redistribution_files_only/economicanalysis.xlsx
+++ b/PVBatterySystem/for_redistribution_files_only/economicanalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\NREL\PVTesBattery\PVBatterySystem\for_redistribution_files_only\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C0C8F3-66E3-461E-974E-D142CF5ADEE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9277B2B-4664-43E0-9945-1F531631EE09}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="17280" windowHeight="9030" firstSheet="4" activeTab="7" xr2:uid="{A1D91E46-10FA-4AC4-B06A-F6A502160249}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="17280" windowHeight="9030" firstSheet="4" activeTab="7" xr2:uid="{C1E708E2-4521-417B-8EC1-39AE1DEC2E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="LCOE System" sheetId="2" r:id="rId1"/>
@@ -383,7 +383,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6129168C-7781-4C11-B05B-2DB9F4D53099}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4283BFB-E3A1-4EB1-A1DF-AF4DE43557D5}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -550,7 +550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F0DDA0-7E23-4D54-895C-32B300699972}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0979630-743B-44E8-B0A6-63CA7FE57A8E}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -717,7 +717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C463E2C5-584C-49AE-8412-7E4B5E088497}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7828797F-AAF7-4830-B613-CE05F298FD05}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -884,7 +884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71267C37-33E9-4310-B3C5-66927D6C2594}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F597D41B-473F-4A3A-A6AF-D72993ACFC0B}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1051,7 +1051,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C906BF18-1284-40FD-90D9-143FDC895F6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC828193-255C-4CA7-BF6E-87264ACE405A}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1218,7 +1218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9089070F-18C3-4843-ACCB-EEA92B7672D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2265ED44-86C5-4C03-92DA-0053FFC16848}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1385,7 +1385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55051659-C976-4196-9061-17B91E0C2515}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D43A7A7-3E8B-4F65-A6F2-948DD47715A8}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1552,7 +1552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085BA460-5E28-4246-B87F-7C13E4A1736F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BBCAA8-625C-4678-BEB2-0BB89A45F72F}">
   <dimension ref="A1:AX1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>